<commit_message>
SCRUM-104 Updated Admin Feature test cases
</commit_message>
<xml_diff>
--- a/Testing/TestCases_Admin.xlsx
+++ b/Testing/TestCases_Admin.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arsan\OneDrive\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\Car-Purchasing\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482291CA-BFFC-4A47-ADF2-793BA3A10145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7632"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,9 +48,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>SRS_ID</t>
   </si>
   <si>
@@ -145,10 +143,6 @@
     <t>email: "namedomain.com"</t>
   </si>
   <si>
-    <t>The field reject the email and display
-"invalid emain"</t>
-  </si>
-  <si>
     <t>SRS_170</t>
   </si>
   <si>
@@ -273,12 +267,18 @@
   <si>
     <t>Email: "omar@gmail.com"
 password: "Ab@123456789"</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>The field reject the email and field becomes red</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -729,33 +729,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A19"/>
+    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" customWidth="1"/>
-    <col min="5" max="5" width="45.88671875" customWidth="1"/>
-    <col min="6" max="6" width="46.6640625" customWidth="1"/>
-    <col min="7" max="7" width="38.88671875" customWidth="1"/>
-    <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="9" width="25.88671875" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" customWidth="1"/>
+    <col min="6" max="6" width="46.7109375" customWidth="1"/>
+    <col min="7" max="7" width="38.85546875" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -779,458 +779,458 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="H9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="F10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="I13" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="D14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>7</v>
+      <c r="H14" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>7</v>
+      <c r="H15" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>7</v>
+      <c r="H16" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>7</v>
+      <c r="H17" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>7</v>
+      <c r="H18" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>7</v>
+      <c r="H19" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1250,7 +1250,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I19" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Passed,Failed,Pending"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>